<commit_message>
update data update last updated
</commit_message>
<xml_diff>
--- a/Resources/Datasets/IsraelData/IsraelStatus.xlsx
+++ b/Resources/Datasets/IsraelData/IsraelStatus.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G94"/>
+  <dimension ref="A1:G96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -803,10 +803,10 @@
         <v>43873</v>
       </c>
       <c r="B19" t="n">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -826,10 +826,10 @@
         <v>43874</v>
       </c>
       <c r="B20" t="n">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C20" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -849,10 +849,10 @@
         <v>43875</v>
       </c>
       <c r="B21" t="n">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C21" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -872,10 +872,10 @@
         <v>43876</v>
       </c>
       <c r="B22" t="n">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C22" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -895,10 +895,10 @@
         <v>43877</v>
       </c>
       <c r="B23" t="n">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C23" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -918,10 +918,10 @@
         <v>43878</v>
       </c>
       <c r="B24" t="n">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C24" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -941,10 +941,10 @@
         <v>43879</v>
       </c>
       <c r="B25" t="n">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C25" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
@@ -964,10 +964,10 @@
         <v>43880</v>
       </c>
       <c r="B26" t="n">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C26" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -987,10 +987,10 @@
         <v>43881</v>
       </c>
       <c r="B27" t="n">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C27" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
@@ -1010,10 +1010,10 @@
         <v>43882</v>
       </c>
       <c r="B28" t="n">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C28" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D28" t="n">
         <v>2</v>
@@ -1033,10 +1033,10 @@
         <v>43883</v>
       </c>
       <c r="B29" t="n">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C29" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D29" t="n">
         <v>2</v>
@@ -1056,10 +1056,10 @@
         <v>43884</v>
       </c>
       <c r="B30" t="n">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C30" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D30" t="n">
         <v>2</v>
@@ -1079,10 +1079,10 @@
         <v>43885</v>
       </c>
       <c r="B31" t="n">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C31" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D31" t="n">
         <v>2</v>
@@ -1102,10 +1102,10 @@
         <v>43886</v>
       </c>
       <c r="B32" t="n">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="C32" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D32" t="n">
         <v>2</v>
@@ -1125,10 +1125,10 @@
         <v>43887</v>
       </c>
       <c r="B33" t="n">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="C33" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D33" t="n">
         <v>2</v>
@@ -1148,10 +1148,10 @@
         <v>43888</v>
       </c>
       <c r="B34" t="n">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="C34" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D34" t="n">
         <v>3</v>
@@ -1171,10 +1171,10 @@
         <v>43889</v>
       </c>
       <c r="B35" t="n">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="C35" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D35" t="n">
         <v>5</v>
@@ -1194,10 +1194,10 @@
         <v>43890</v>
       </c>
       <c r="B36" t="n">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="C36" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D36" t="n">
         <v>5</v>
@@ -1217,10 +1217,10 @@
         <v>43891</v>
       </c>
       <c r="B37" t="n">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="C37" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D37" t="n">
         <v>7</v>
@@ -1240,10 +1240,10 @@
         <v>43892</v>
       </c>
       <c r="B38" t="n">
-        <v>1633</v>
+        <v>1631</v>
       </c>
       <c r="C38" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D38" t="n">
         <v>11</v>
@@ -1263,10 +1263,10 @@
         <v>43893</v>
       </c>
       <c r="B39" t="n">
-        <v>1867</v>
+        <v>1865</v>
       </c>
       <c r="C39" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D39" t="n">
         <v>11</v>
@@ -1286,10 +1286,10 @@
         <v>43894</v>
       </c>
       <c r="B40" t="n">
-        <v>1996</v>
+        <v>1994</v>
       </c>
       <c r="C40" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D40" t="n">
         <v>11</v>
@@ -1309,10 +1309,10 @@
         <v>43895</v>
       </c>
       <c r="B41" t="n">
-        <v>2169</v>
+        <v>2167</v>
       </c>
       <c r="C41" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D41" t="n">
         <v>13</v>
@@ -1332,10 +1332,10 @@
         <v>43896</v>
       </c>
       <c r="B42" t="n">
-        <v>2444</v>
+        <v>2442</v>
       </c>
       <c r="C42" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D42" t="n">
         <v>16</v>
@@ -1355,10 +1355,10 @@
         <v>43897</v>
       </c>
       <c r="B43" t="n">
-        <v>2782</v>
+        <v>2780</v>
       </c>
       <c r="C43" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D43" t="n">
         <v>19</v>
@@ -1378,10 +1378,10 @@
         <v>43898</v>
       </c>
       <c r="B44" t="n">
-        <v>3204</v>
+        <v>3202</v>
       </c>
       <c r="C44" t="n">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D44" t="n">
         <v>26</v>
@@ -1401,10 +1401,10 @@
         <v>43899</v>
       </c>
       <c r="B45" t="n">
-        <v>3723</v>
+        <v>3721</v>
       </c>
       <c r="C45" t="n">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D45" t="n">
         <v>40</v>
@@ -1424,10 +1424,10 @@
         <v>43900</v>
       </c>
       <c r="B46" t="n">
-        <v>4244</v>
+        <v>4242</v>
       </c>
       <c r="C46" t="n">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D46" t="n">
         <v>59</v>
@@ -1447,10 +1447,10 @@
         <v>43901</v>
       </c>
       <c r="B47" t="n">
-        <v>4647</v>
+        <v>4645</v>
       </c>
       <c r="C47" t="n">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D47" t="n">
         <v>81</v>
@@ -1470,10 +1470,10 @@
         <v>43902</v>
       </c>
       <c r="B48" t="n">
-        <v>5254</v>
+        <v>5252</v>
       </c>
       <c r="C48" t="n">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D48" t="n">
         <v>103</v>
@@ -1493,10 +1493,10 @@
         <v>43903</v>
       </c>
       <c r="B49" t="n">
-        <v>5950</v>
+        <v>5948</v>
       </c>
       <c r="C49" t="n">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D49" t="n">
         <v>123</v>
@@ -1516,10 +1516,10 @@
         <v>43904</v>
       </c>
       <c r="B50" t="n">
-        <v>6563</v>
+        <v>6561</v>
       </c>
       <c r="C50" t="n">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D50" t="n">
         <v>161</v>
@@ -1539,10 +1539,10 @@
         <v>43905</v>
       </c>
       <c r="B51" t="n">
-        <v>7747</v>
+        <v>7745</v>
       </c>
       <c r="C51" t="n">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D51" t="n">
         <v>201</v>
@@ -1562,10 +1562,10 @@
         <v>43906</v>
       </c>
       <c r="B52" t="n">
-        <v>9092</v>
+        <v>9090</v>
       </c>
       <c r="C52" t="n">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D52" t="n">
         <v>221</v>
@@ -1585,10 +1585,10 @@
         <v>43907</v>
       </c>
       <c r="B53" t="n">
-        <v>10748</v>
+        <v>10747</v>
       </c>
       <c r="C53" t="n">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D53" t="n">
         <v>257</v>
@@ -1634,7 +1634,7 @@
         <v>14947</v>
       </c>
       <c r="C55" t="n">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="D55" t="n">
         <v>295</v>
@@ -1657,7 +1657,7 @@
         <v>17272</v>
       </c>
       <c r="C56" t="n">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="D56" t="n">
         <v>288</v>
@@ -1680,7 +1680,7 @@
         <v>19369</v>
       </c>
       <c r="C57" t="n">
-        <v>1022</v>
+        <v>1026</v>
       </c>
       <c r="D57" t="n">
         <v>276</v>
@@ -1703,7 +1703,7 @@
         <v>22705</v>
       </c>
       <c r="C58" t="n">
-        <v>1271</v>
+        <v>1275</v>
       </c>
       <c r="D58" t="n">
         <v>323</v>
@@ -1726,7 +1726,7 @@
         <v>26335</v>
       </c>
       <c r="C59" t="n">
-        <v>1619</v>
+        <v>1623</v>
       </c>
       <c r="D59" t="n">
         <v>350</v>
@@ -1749,7 +1749,7 @@
         <v>31118</v>
       </c>
       <c r="C60" t="n">
-        <v>2041</v>
+        <v>2046</v>
       </c>
       <c r="D60" t="n">
         <v>393</v>
@@ -1772,7 +1772,7 @@
         <v>37044</v>
       </c>
       <c r="C61" t="n">
-        <v>2465</v>
+        <v>2471</v>
       </c>
       <c r="D61" t="n">
         <v>412</v>
@@ -1795,7 +1795,7 @@
         <v>43555</v>
       </c>
       <c r="C62" t="n">
-        <v>2992</v>
+        <v>2998</v>
       </c>
       <c r="D62" t="n">
         <v>464</v>
@@ -1815,10 +1815,10 @@
         <v>43917</v>
       </c>
       <c r="B63" t="n">
-        <v>49300</v>
+        <v>49299</v>
       </c>
       <c r="C63" t="n">
-        <v>3427</v>
+        <v>3434</v>
       </c>
       <c r="D63" t="n">
         <v>515</v>
@@ -1841,7 +1841,7 @@
         <v>55010</v>
       </c>
       <c r="C64" t="n">
-        <v>3907</v>
+        <v>3916</v>
       </c>
       <c r="D64" t="n">
         <v>512</v>
@@ -1864,7 +1864,7 @@
         <v>62574</v>
       </c>
       <c r="C65" t="n">
-        <v>4439</v>
+        <v>4452</v>
       </c>
       <c r="D65" t="n">
         <v>541</v>
@@ -1887,7 +1887,7 @@
         <v>69665</v>
       </c>
       <c r="C66" t="n">
-        <v>4984</v>
+        <v>4999</v>
       </c>
       <c r="D66" t="n">
         <v>617</v>
@@ -1910,7 +1910,7 @@
         <v>77625</v>
       </c>
       <c r="C67" t="n">
-        <v>5713</v>
+        <v>5732</v>
       </c>
       <c r="D67" t="n">
         <v>665</v>
@@ -1933,7 +1933,7 @@
         <v>86606</v>
       </c>
       <c r="C68" t="n">
-        <v>6407</v>
+        <v>6428</v>
       </c>
       <c r="D68" t="n">
         <v>767</v>
@@ -1956,7 +1956,7 @@
         <v>96823</v>
       </c>
       <c r="C69" t="n">
-        <v>7127</v>
+        <v>7150</v>
       </c>
       <c r="D69" t="n">
         <v>811</v>
@@ -1979,7 +1979,7 @@
         <v>107148</v>
       </c>
       <c r="C70" t="n">
-        <v>7726</v>
+        <v>7748</v>
       </c>
       <c r="D70" t="n">
         <v>800</v>
@@ -2002,7 +2002,7 @@
         <v>113664</v>
       </c>
       <c r="C71" t="n">
-        <v>8154</v>
+        <v>8176</v>
       </c>
       <c r="D71" t="n">
         <v>786</v>
@@ -2014,7 +2014,7 @@
         <v>107</v>
       </c>
       <c r="G71" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="72">
@@ -2025,7 +2025,7 @@
         <v>123107</v>
       </c>
       <c r="C72" t="n">
-        <v>8733</v>
+        <v>8755</v>
       </c>
       <c r="D72" t="n">
         <v>823</v>
@@ -2037,7 +2037,7 @@
         <v>106</v>
       </c>
       <c r="G72" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="73">
@@ -2045,10 +2045,10 @@
         <v>43927</v>
       </c>
       <c r="B73" t="n">
-        <v>130604</v>
+        <v>130603</v>
       </c>
       <c r="C73" t="n">
-        <v>9185</v>
+        <v>9206</v>
       </c>
       <c r="D73" t="n">
         <v>806</v>
@@ -2060,7 +2060,7 @@
         <v>110</v>
       </c>
       <c r="G73" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="74">
@@ -2068,10 +2068,10 @@
         <v>43928</v>
       </c>
       <c r="B74" t="n">
-        <v>137532</v>
+        <v>137531</v>
       </c>
       <c r="C74" t="n">
-        <v>9564</v>
+        <v>9585</v>
       </c>
       <c r="D74" t="n">
         <v>743</v>
@@ -2083,7 +2083,7 @@
         <v>106</v>
       </c>
       <c r="G74" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75">
@@ -2091,10 +2091,10 @@
         <v>43929</v>
       </c>
       <c r="B75" t="n">
-        <v>143402</v>
+        <v>143401</v>
       </c>
       <c r="C75" t="n">
-        <v>9902</v>
+        <v>9925</v>
       </c>
       <c r="D75" t="n">
         <v>690</v>
@@ -2106,7 +2106,7 @@
         <v>114</v>
       </c>
       <c r="G75" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76">
@@ -2114,10 +2114,10 @@
         <v>43930</v>
       </c>
       <c r="B76" t="n">
-        <v>149150</v>
+        <v>149149</v>
       </c>
       <c r="C76" t="n">
-        <v>10246</v>
+        <v>10269</v>
       </c>
       <c r="D76" t="n">
         <v>663</v>
@@ -2129,7 +2129,7 @@
         <v>117</v>
       </c>
       <c r="G76" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="77">
@@ -2140,7 +2140,7 @@
         <v>156476</v>
       </c>
       <c r="C77" t="n">
-        <v>10607</v>
+        <v>10629</v>
       </c>
       <c r="D77" t="n">
         <v>666</v>
@@ -2152,7 +2152,7 @@
         <v>128</v>
       </c>
       <c r="G77" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="78">
@@ -2163,7 +2163,7 @@
         <v>163167</v>
       </c>
       <c r="C78" t="n">
-        <v>10952</v>
+        <v>10974</v>
       </c>
       <c r="D78" t="n">
         <v>623</v>
@@ -2175,7 +2175,7 @@
         <v>130</v>
       </c>
       <c r="G78" t="n">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="79">
@@ -2183,10 +2183,10 @@
         <v>43933</v>
       </c>
       <c r="B79" t="n">
-        <v>173787</v>
+        <v>173789</v>
       </c>
       <c r="C79" t="n">
-        <v>11510</v>
+        <v>11534</v>
       </c>
       <c r="D79" t="n">
         <v>664</v>
@@ -2198,7 +2198,7 @@
         <v>130</v>
       </c>
       <c r="G79" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="80">
@@ -2206,10 +2206,10 @@
         <v>43934</v>
       </c>
       <c r="B80" t="n">
-        <v>184746</v>
+        <v>184748</v>
       </c>
       <c r="C80" t="n">
-        <v>11954</v>
+        <v>11978</v>
       </c>
       <c r="D80" t="n">
         <v>684</v>
@@ -2221,7 +2221,7 @@
         <v>137</v>
       </c>
       <c r="G80" t="n">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="81">
@@ -2229,10 +2229,10 @@
         <v>43935</v>
       </c>
       <c r="B81" t="n">
-        <v>197409</v>
+        <v>197411</v>
       </c>
       <c r="C81" t="n">
-        <v>12361</v>
+        <v>12383</v>
       </c>
       <c r="D81" t="n">
         <v>672</v>
@@ -2244,7 +2244,7 @@
         <v>135</v>
       </c>
       <c r="G81" t="n">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="82">
@@ -2252,10 +2252,10 @@
         <v>43936</v>
       </c>
       <c r="B82" t="n">
-        <v>206859</v>
+        <v>206861</v>
       </c>
       <c r="C82" t="n">
-        <v>12673</v>
+        <v>12694</v>
       </c>
       <c r="D82" t="n">
         <v>670</v>
@@ -2267,7 +2267,7 @@
         <v>132</v>
       </c>
       <c r="G82" t="n">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="83">
@@ -2275,22 +2275,22 @@
         <v>43937</v>
       </c>
       <c r="B83" t="n">
-        <v>219643</v>
+        <v>219645</v>
       </c>
       <c r="C83" t="n">
-        <v>12974</v>
+        <v>12995</v>
       </c>
       <c r="D83" t="n">
         <v>703</v>
       </c>
       <c r="E83" t="n">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F83" t="n">
         <v>136</v>
       </c>
       <c r="G83" t="n">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="84">
@@ -2298,10 +2298,10 @@
         <v>43938</v>
       </c>
       <c r="B84" t="n">
-        <v>231204</v>
+        <v>231206</v>
       </c>
       <c r="C84" t="n">
-        <v>13275</v>
+        <v>13295</v>
       </c>
       <c r="D84" t="n">
         <v>662</v>
@@ -2313,7 +2313,7 @@
         <v>125</v>
       </c>
       <c r="G84" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="85">
@@ -2321,10 +2321,10 @@
         <v>43939</v>
       </c>
       <c r="B85" t="n">
-        <v>241834</v>
+        <v>241836</v>
       </c>
       <c r="C85" t="n">
-        <v>13585</v>
+        <v>13605</v>
       </c>
       <c r="D85" t="n">
         <v>642</v>
@@ -2336,7 +2336,7 @@
         <v>117</v>
       </c>
       <c r="G85" t="n">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="86">
@@ -2344,10 +2344,10 @@
         <v>43940</v>
       </c>
       <c r="B86" t="n">
-        <v>253297</v>
+        <v>253299</v>
       </c>
       <c r="C86" t="n">
-        <v>13878</v>
+        <v>13896</v>
       </c>
       <c r="D86" t="n">
         <v>619</v>
@@ -2359,7 +2359,7 @@
         <v>117</v>
       </c>
       <c r="G86" t="n">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="87">
@@ -2367,10 +2367,10 @@
         <v>43941</v>
       </c>
       <c r="B87" t="n">
-        <v>268644</v>
+        <v>268646</v>
       </c>
       <c r="C87" t="n">
-        <v>14185</v>
+        <v>14199</v>
       </c>
       <c r="D87" t="n">
         <v>614</v>
@@ -2382,7 +2382,7 @@
         <v>122</v>
       </c>
       <c r="G87" t="n">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="88">
@@ -2390,10 +2390,10 @@
         <v>43942</v>
       </c>
       <c r="B88" t="n">
-        <v>282229</v>
+        <v>282231</v>
       </c>
       <c r="C88" t="n">
-        <v>14479</v>
+        <v>14491</v>
       </c>
       <c r="D88" t="n">
         <v>543</v>
@@ -2405,7 +2405,7 @@
         <v>117</v>
       </c>
       <c r="G88" t="n">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="89">
@@ -2413,10 +2413,10 @@
         <v>43943</v>
       </c>
       <c r="B89" t="n">
-        <v>295523</v>
+        <v>295525</v>
       </c>
       <c r="C89" t="n">
-        <v>14708</v>
+        <v>14720</v>
       </c>
       <c r="D89" t="n">
         <v>532</v>
@@ -2428,7 +2428,7 @@
         <v>108</v>
       </c>
       <c r="G89" t="n">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="90">
@@ -2436,10 +2436,10 @@
         <v>43944</v>
       </c>
       <c r="B90" t="n">
-        <v>309680</v>
+        <v>309683</v>
       </c>
       <c r="C90" t="n">
-        <v>14989</v>
+        <v>15000</v>
       </c>
       <c r="D90" t="n">
         <v>491</v>
@@ -2451,7 +2451,7 @@
         <v>112</v>
       </c>
       <c r="G90" t="n">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="91">
@@ -2459,10 +2459,10 @@
         <v>43945</v>
       </c>
       <c r="B91" t="n">
-        <v>322293</v>
+        <v>322296</v>
       </c>
       <c r="C91" t="n">
-        <v>15243</v>
+        <v>15255</v>
       </c>
       <c r="D91" t="n">
         <v>454</v>
@@ -2474,7 +2474,7 @@
         <v>104</v>
       </c>
       <c r="G91" t="n">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="92">
@@ -2482,10 +2482,10 @@
         <v>43946</v>
       </c>
       <c r="B92" t="n">
-        <v>331372</v>
+        <v>331374</v>
       </c>
       <c r="C92" t="n">
-        <v>15403</v>
+        <v>15415</v>
       </c>
       <c r="D92" t="n">
         <v>432</v>
@@ -2497,7 +2497,7 @@
         <v>104</v>
       </c>
       <c r="G92" t="n">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93">
@@ -2505,10 +2505,10 @@
         <v>43947</v>
       </c>
       <c r="B93" t="n">
-        <v>339839</v>
+        <v>339841</v>
       </c>
       <c r="C93" t="n">
-        <v>15491</v>
+        <v>15503</v>
       </c>
       <c r="D93" t="n">
         <v>441</v>
@@ -2520,7 +2520,7 @@
         <v>109</v>
       </c>
       <c r="G93" t="n">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="94">
@@ -2528,10 +2528,10 @@
         <v>43948</v>
       </c>
       <c r="B94" t="n">
-        <v>350858</v>
+        <v>350860</v>
       </c>
       <c r="C94" t="n">
-        <v>15607</v>
+        <v>15618</v>
       </c>
       <c r="D94" t="n">
         <v>410</v>
@@ -2543,7 +2543,53 @@
         <v>99</v>
       </c>
       <c r="G94" t="n">
-        <v>205</v>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="n">
+        <v>43949</v>
+      </c>
+      <c r="B95" t="n">
+        <v>361501</v>
+      </c>
+      <c r="C95" t="n">
+        <v>15786</v>
+      </c>
+      <c r="D95" t="n">
+        <v>391</v>
+      </c>
+      <c r="E95" t="n">
+        <v>125</v>
+      </c>
+      <c r="F95" t="n">
+        <v>98</v>
+      </c>
+      <c r="G95" t="n">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="n">
+        <v>43950</v>
+      </c>
+      <c r="B96" t="n">
+        <v>370505</v>
+      </c>
+      <c r="C96" t="n">
+        <v>15869</v>
+      </c>
+      <c r="D96" t="n">
+        <v>370</v>
+      </c>
+      <c r="E96" t="n">
+        <v>118</v>
+      </c>
+      <c r="F96" t="n">
+        <v>93</v>
+      </c>
+      <c r="G96" t="n">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>